<commit_message>
Domain osa tehtud, nüüd tulevad repositooriumid
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E96CB4-7889-4FB3-907F-F0AE07C2ED56}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B8EEFF-3F6C-4321-B49E-25539430E699}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="45">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Kodutöö 2. osa</t>
+  </si>
+  <si>
+    <t>Kodutöö 3. osa</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1006,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1163,7 +1166,9 @@
       <c r="C9" s="8">
         <v>0.77083333333333337</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="8">
+        <v>0.84722222222222221</v>
+      </c>
       <c r="E9" s="6"/>
       <c r="F9" s="5"/>
       <c r="G9" s="6" t="s">
@@ -1177,12 +1182,18 @@
       <c r="A10" s="9">
         <v>4</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="7">
+        <v>43883</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.31597222222222221</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="6"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>

</xml_diff>

<commit_message>
quantity db context muudetud, minut 43, 3osa
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F5071B-E225-4E7C-A435-82481F7C61E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD78A6A-4DB8-4CA3-A342-CD8B42E1A8A1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="46">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Kodutöö 3. osa</t>
+  </si>
+  <si>
+    <t>minut 28</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1009,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1208,13 +1211,17 @@
       <c r="C11" s="8">
         <v>0.70138888888888884</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="8">
+        <v>0.72291666666666676</v>
+      </c>
       <c r="E11" s="6"/>
       <c r="F11" s="5"/>
       <c r="G11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="31"/>
+      <c r="H11" s="31" t="s">
+        <v>45</v>
+      </c>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
@@ -1223,11 +1230,15 @@
         <v>6</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
+      <c r="C12" s="8">
+        <v>0.53472222222222221</v>
+      </c>
       <c r="D12" s="8"/>
       <c r="E12" s="6"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>

</xml_diff>

<commit_message>
infra ja startup muudetud, 1h vd, 3osa
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD78A6A-4DB8-4CA3-A342-CD8B42E1A8A1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76116E7-678B-4061-986B-56B0796FC5E4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="47">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>minut 28</t>
+  </si>
+  <si>
+    <t>lahuta 30min</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1012,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1239,7 +1242,9 @@
       <c r="G12" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="6"/>
+      <c r="H12" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>

</xml_diff>

<commit_message>
delete osa tehtud 3.osa
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76116E7-678B-4061-986B-56B0796FC5E4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01909A96-1CF2-4F62-83AD-D6BA9791A46A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="48">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>lahuta 30min</t>
+  </si>
+  <si>
+    <t>Kodutöö 3. osa + laadisin resharperi uuesti alla</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1015,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1240,7 +1243,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="5"/>
       <c r="G12" s="6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
3. osa tehtud, ilma erroriteta, kõik töötab
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01909A96-1CF2-4F62-83AD-D6BA9791A46A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE952E8-51C0-4F51-92C4-27E4957E470F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -169,12 +169,6 @@
   </si>
   <si>
     <t>Kodutöö 3. osa</t>
-  </si>
-  <si>
-    <t>minut 28</t>
-  </si>
-  <si>
-    <t>lahuta 30min</t>
   </si>
   <si>
     <t>Kodutöö 3. osa + laadisin resharperi uuesti alla</t>
@@ -1015,7 +1009,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1135,7 +1129,9 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5">
+        <v>155</v>
+      </c>
       <c r="G7" s="6" t="s">
         <v>41</v>
       </c>
@@ -1179,7 +1175,9 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5">
+        <v>110</v>
+      </c>
       <c r="G9" s="6" t="s">
         <v>43</v>
       </c>
@@ -1201,7 +1199,9 @@
         <v>0.375</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5">
+        <v>85</v>
+      </c>
       <c r="G10" s="6" t="s">
         <v>44</v>
       </c>
@@ -1221,13 +1221,13 @@
         <v>0.72291666666666676</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
+      <c r="F11" s="5">
+        <v>31</v>
+      </c>
       <c r="G11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="31" t="s">
-        <v>45</v>
-      </c>
+      <c r="H11" s="31"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
@@ -1239,15 +1239,17 @@
       <c r="C12" s="8">
         <v>0.53472222222222221</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="8">
+        <v>0.72222222222222221</v>
+      </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="5"/>
+      <c r="F12" s="5">
+        <v>270</v>
+      </c>
       <c r="G12" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>
@@ -1345,7 +1347,7 @@
       <c r="E19" s="43"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>66</v>
+        <v>717</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>
@@ -1365,7 +1367,7 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
html failid tehtud lühemaks kasutades extensioneid 52 minut 4. osa
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE952E8-51C0-4F51-92C4-27E4957E470F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DACB25C-1AA1-45D6-8E3E-B84254AA96CC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="47">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>Kodutöö 3. osa + laadisin resharperi uuesti alla</t>
+  </si>
+  <si>
+    <t>Kodutöö 4. osa</t>
   </si>
 </sst>
 </file>
@@ -1235,7 +1238,9 @@
       <c r="A12" s="9">
         <v>6</v>
       </c>
-      <c r="B12" s="7"/>
+      <c r="B12" s="7">
+        <v>43884</v>
+      </c>
       <c r="C12" s="8">
         <v>0.53472222222222221</v>
       </c>
@@ -1258,11 +1263,15 @@
         <v>7</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
+      <c r="C13" s="8">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="D13" s="8"/>
       <c r="E13" s="6"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
+      <c r="G13" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>

</xml_diff>

<commit_message>
VIGADEGA COMMIT: 1. Edit ja Create lehed näevad lappes välja 2. Valid From displayb ennast 2x 3. Index.cshtml.cs ei leia üles db, seega ei tea kas sortimine hakkas tööle.
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DACB25C-1AA1-45D6-8E3E-B84254AA96CC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0DD818-98D7-46B1-A0C6-DED7F5EC0A5B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="48">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>Kodutöö 4. osa</t>
+  </si>
+  <si>
+    <t>Kodutöö 5. osa</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1015,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1266,9 +1269,13 @@
       <c r="C13" s="8">
         <v>0.72916666666666663</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="8">
+        <v>0.82291666666666663</v>
+      </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="5">
+        <v>135</v>
+      </c>
       <c r="G13" s="6" t="s">
         <v>46</v>
       </c>
@@ -1281,11 +1288,19 @@
         <v>8</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="8">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.86805555555555547</v>
+      </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
+      <c r="F14" s="5">
+        <v>60</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
@@ -1356,7 +1371,7 @@
       <c r="E19" s="43"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>717</v>
+        <v>912</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
errorid eemaldatud, 5. osa k.a kõik õige
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0DD818-98D7-46B1-A0C6-DED7F5EC0A5B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69E3FA1-880A-4492-AF16-9033F72320ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Nädal 4" sheetId="6" r:id="rId1"/>
-    <sheet name="Nädal 3" sheetId="5" r:id="rId2"/>
-    <sheet name="Nädal 2" sheetId="3" r:id="rId3"/>
-    <sheet name="Nädal 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Nädal 5" sheetId="7" r:id="rId1"/>
+    <sheet name="Nädal 4" sheetId="6" r:id="rId2"/>
+    <sheet name="Nädal 3" sheetId="5" r:id="rId3"/>
+    <sheet name="Nädal 2" sheetId="3" r:id="rId4"/>
+    <sheet name="Nädal 1" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="50">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -178,6 +179,12 @@
   </si>
   <si>
     <t>Kodutöö 5. osa</t>
+  </si>
+  <si>
+    <t>Kodutöö 6. osa</t>
+  </si>
+  <si>
+    <t>5. osa errorite eemaldamine</t>
   </si>
 </sst>
 </file>
@@ -1011,11 +1018,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4BA9E6-34DD-4C1C-AEEF-5A72BA45E7B5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8ACF002-C02F-4F6D-A9DF-5CDFC75330FF}">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1073,7 +1080,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="53">
-        <v>43877</v>
+        <v>43888</v>
       </c>
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
@@ -1126,20 +1133,20 @@
         <v>1</v>
       </c>
       <c r="B7" s="7">
-        <v>43881</v>
+        <v>43886</v>
       </c>
       <c r="C7" s="8">
-        <v>0.78125</v>
+        <v>0.3923611111111111</v>
       </c>
       <c r="D7" s="8">
-        <v>0.88888888888888884</v>
+        <v>0.40972222222222227</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="5">
-        <v>155</v>
+        <v>25</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="20"/>
@@ -1151,17 +1158,13 @@
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="38">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D8" s="38">
-        <v>0.37916666666666665</v>
-      </c>
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D8" s="38"/>
       <c r="E8" s="39"/>
-      <c r="F8" s="40">
-        <v>66</v>
-      </c>
+      <c r="F8" s="40"/>
       <c r="G8" s="39" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H8" s="39"/>
       <c r="I8" s="6"/>
@@ -1171,22 +1174,12 @@
       <c r="A9" s="9">
         <v>3</v>
       </c>
-      <c r="B9" s="37">
-        <v>43882</v>
-      </c>
-      <c r="C9" s="8">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0.84722222222222221</v>
-      </c>
+      <c r="B9" s="37"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="5">
-        <v>110</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
@@ -1195,22 +1188,12 @@
       <c r="A10" s="9">
         <v>4</v>
       </c>
-      <c r="B10" s="7">
-        <v>43883</v>
-      </c>
-      <c r="C10" s="8">
-        <v>0.31597222222222221</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0.375</v>
-      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="5">
-        <v>85</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>44</v>
-      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
@@ -1220,19 +1203,11 @@
         <v>5</v>
       </c>
       <c r="B11" s="7"/>
-      <c r="C11" s="8">
-        <v>0.70138888888888884</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0.72291666666666676</v>
-      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="5">
-        <v>31</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>44</v>
-      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
       <c r="H11" s="31"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
@@ -1241,22 +1216,12 @@
       <c r="A12" s="9">
         <v>6</v>
       </c>
-      <c r="B12" s="7">
-        <v>43884</v>
-      </c>
-      <c r="C12" s="8">
-        <v>0.53472222222222221</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0.72222222222222221</v>
-      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="5">
-        <v>270</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
@@ -1266,19 +1231,11 @@
         <v>7</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="8">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="D13" s="8">
-        <v>0.82291666666666663</v>
-      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="5">
-        <v>135</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>46</v>
-      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
@@ -1288,19 +1245,11 @@
         <v>8</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="8">
-        <v>0.82638888888888884</v>
-      </c>
-      <c r="D14" s="8">
-        <v>0.86805555555555547</v>
-      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="5">
-        <v>60</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>47</v>
-      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
@@ -1371,7 +1320,7 @@
       <c r="E19" s="43"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>912</v>
+        <v>25</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>
@@ -1396,6 +1345,391 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4BA9E6-34DD-4C1C-AEEF-5A72BA45E7B5}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.36328125" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
+    <col min="6" max="6" width="6.54296875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="43.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.453125" customWidth="1"/>
+    <col min="10" max="10" width="3.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="46"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="47"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="49"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="51"/>
+      <c r="C4" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="53">
+        <v>43884</v>
+      </c>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="54"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="57"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="59"/>
+      <c r="C6" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="17">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7">
+        <v>43881</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.78125</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5">
+        <v>155</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="38">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D8" s="38">
+        <v>0.37916666666666665</v>
+      </c>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40">
+        <v>66</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="39"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="37">
+        <v>43882</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5">
+        <v>110</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7">
+        <v>43883</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.31597222222222221</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5">
+        <v>85</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.72291666666666676</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5">
+        <v>31</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="31"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="9">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7">
+        <v>43884</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5">
+        <v>270</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="9">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5">
+        <v>135</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.86805555555555547</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5">
+        <v>60</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="9">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="9">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="9">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="23">
+        <v>12</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="30">
+        <f>SUM(F7:F18)</f>
+        <v>912</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8DD912-1C37-45A7-B4D1-E4B8ABC30324}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -1756,7 +2090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CFBBF56-839A-44F9-A412-7D1F721290A1}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -2179,7 +2513,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L19"/>
   <sheetViews>

</xml_diff>

<commit_message>
7. osa tehtud, kõik töötab.
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5355D5D6-7013-4F67-9D5E-4CB5F583323E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA59333A-7679-4618-A89A-71BCD083BCC9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="51">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>5. osa errorite eemaldamine</t>
+  </si>
+  <si>
+    <t>Kodutöö 7. osa</t>
   </si>
 </sst>
 </file>
@@ -1022,7 +1025,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1179,11 +1182,19 @@
         <v>3</v>
       </c>
       <c r="B9" s="37"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="C9" s="8">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.8125</v>
+      </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
+      <c r="F9" s="5">
+        <v>70</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
@@ -1324,7 +1335,7 @@
       <c r="E19" s="43"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>57</v>
+        <v>127</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
base klass loodud, 9 osa tehtud
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CDC8C2-95FB-426E-B1FA-C812A3776F8F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DD0E07-9539-4690-B7A1-F345AF5DDD24}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="53">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>Kodutöö 8. osa</t>
+  </si>
+  <si>
+    <t>Kodutöö 9-10. osa</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1031,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1208,11 +1211,15 @@
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="8">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="D10" s="8"/>
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.88263888888888886</v>
+      </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5">
+        <v>61</v>
+      </c>
       <c r="G10" s="6" t="s">
         <v>51</v>
       </c>
@@ -1224,12 +1231,18 @@
       <c r="A11" s="9">
         <v>5</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="7">
+        <v>43888</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.30555555555555552</v>
+      </c>
       <c r="D11" s="8"/>
       <c r="E11" s="6"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
+      <c r="G11" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="H11" s="31"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
@@ -1342,7 +1355,7 @@
       <c r="E19" s="43"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>127</v>
+        <v>188</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Interfaced loodud ja refaktooritud
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A08C283-3F3C-4A79-A50A-94A458FDE486}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961D599C-BF8C-48E6-9245-179DE2178EBD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="55">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Kodutöö 11. osa</t>
+  </si>
+  <si>
+    <t>Kodutöö 12. osa</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1037,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1264,9 +1267,13 @@
       <c r="C12" s="8">
         <v>0.85416666666666663</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="8">
+        <v>0.90625</v>
+      </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="5"/>
+      <c r="F12" s="5">
+        <v>75</v>
+      </c>
       <c r="G12" s="6" t="s">
         <v>53</v>
       </c>
@@ -1278,12 +1285,18 @@
       <c r="A13" s="9">
         <v>7</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
+      <c r="B13" s="7">
+        <v>43890</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.32569444444444445</v>
+      </c>
       <c r="D13" s="8"/>
       <c r="E13" s="6"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
+      <c r="G13" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
@@ -1368,7 +1381,7 @@
       <c r="E19" s="43"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>453</v>
+        <v>528</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
12. osa tehtud, aga küsib et lisaksi nuue startupi faili.
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961D599C-BF8C-48E6-9245-179DE2178EBD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CE31D4-E8FA-494D-AED3-9A3F71ED3237}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="56">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>Kodutöö 12. osa</t>
+  </si>
+  <si>
+    <t>startup failiga mingi jama</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1040,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1291,13 +1294,19 @@
       <c r="C13" s="8">
         <v>0.32569444444444445</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="8">
+        <v>0.37152777777777773</v>
+      </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="5">
+        <v>66</v>
+      </c>
       <c r="G13" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
@@ -1381,7 +1390,7 @@
       <c r="E19" s="43"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>528</v>
+        <v>594</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
errorid eemaldatud, KÕIK töötab
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CE31D4-E8FA-494D-AED3-9A3F71ED3237}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7704DFB-27BA-444B-900C-3CD3042AFF5C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="57">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>startup failiga mingi jama</t>
+  </si>
+  <si>
+    <t>Errorite elimineerimine</t>
   </si>
 </sst>
 </file>
@@ -1040,7 +1043,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1315,11 +1318,19 @@
         <v>8</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="8">
+        <v>0.40625</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.41319444444444442</v>
+      </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
+      <c r="F14" s="5">
+        <v>10</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
@@ -1390,7 +1401,7 @@
       <c r="E19" s="43"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>594</v>
+        <v>604</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
17. vvideot tehtud, errorid sees. ei ole browseris vaatanud laates 13 videost
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7704DFB-27BA-444B-900C-3CD3042AFF5C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB4B91A-8DB2-4E15-8A0B-8F7D23537EFF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="59">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>Errorite elimineerimine</t>
+  </si>
+  <si>
+    <t>Kodutöö 13. osa</t>
+  </si>
+  <si>
+    <t>Kodutöö 13-17. osa</t>
   </si>
 </sst>
 </file>
@@ -1042,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8ACF002-C02F-4F6D-A9DF-5CDFC75330FF}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1339,12 +1345,20 @@
       <c r="A15" s="9">
         <v>9</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="32"/>
+      <c r="B15" s="7">
+        <v>412785</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="D15" s="32">
+        <v>0.4826388888888889</v>
+      </c>
       <c r="E15" s="6"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
+      <c r="G15" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
@@ -1354,11 +1368,15 @@
         <v>10</v>
       </c>
       <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
+      <c r="C16" s="8">
+        <v>0.69444444444444453</v>
+      </c>
       <c r="D16" s="8"/>
       <c r="E16" s="6"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
+      <c r="G16" s="6" t="s">
+        <v>58</v>
+      </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>

</xml_diff>

<commit_message>
errorid eemaldatud, 17. osa done
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB4B91A-8DB2-4E15-8A0B-8F7D23537EFF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC50EB25-23F7-4924-B6F4-0043CE57DDE1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Nädal 5" sheetId="7" r:id="rId1"/>
-    <sheet name="Nädal 4" sheetId="6" r:id="rId2"/>
-    <sheet name="Nädal 3" sheetId="5" r:id="rId3"/>
-    <sheet name="Nädal 2" sheetId="3" r:id="rId4"/>
-    <sheet name="Nädal 1" sheetId="1" r:id="rId5"/>
+    <sheet name="Nädal 6" sheetId="8" r:id="rId1"/>
+    <sheet name="Nädal 5" sheetId="7" r:id="rId2"/>
+    <sheet name="Nädal 4" sheetId="6" r:id="rId3"/>
+    <sheet name="Nädal 3" sheetId="5" r:id="rId4"/>
+    <sheet name="Nädal 2" sheetId="3" r:id="rId5"/>
+    <sheet name="Nädal 1" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="60">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -212,6 +213,9 @@
   </si>
   <si>
     <t>Kodutöö 13-17. osa</t>
+  </si>
+  <si>
+    <t>Eelmise kodutöö errorite eelimineerimine</t>
   </si>
 </sst>
 </file>
@@ -1045,11 +1049,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8ACF002-C02F-4F6D-A9DF-5CDFC75330FF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D5B9A5-82EB-41D0-B31E-F472544F2A17}">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1160,20 +1164,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="7">
-        <v>43886</v>
+        <v>43892</v>
       </c>
       <c r="C7" s="8">
-        <v>0.3923611111111111</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0.40972222222222227</v>
-      </c>
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D7" s="8"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="5">
-        <v>25</v>
-      </c>
+      <c r="F7" s="5"/>
       <c r="G7" s="6" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="20"/>
@@ -1184,19 +1184,11 @@
         <v>2</v>
       </c>
       <c r="B8" s="7"/>
-      <c r="C8" s="38">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="D8" s="38">
-        <v>0.75138888888888899</v>
-      </c>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="39"/>
-      <c r="F8" s="40">
-        <v>32</v>
-      </c>
-      <c r="G8" s="39" t="s">
-        <v>48</v>
-      </c>
+      <c r="F8" s="40"/>
+      <c r="G8" s="39"/>
       <c r="H8" s="39"/>
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
@@ -1206,19 +1198,11 @@
         <v>3</v>
       </c>
       <c r="B9" s="37"/>
-      <c r="C9" s="8">
-        <v>0.76388888888888884</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0.8125</v>
-      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="5">
-        <v>70</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
@@ -1228,19 +1212,11 @@
         <v>4</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="8">
-        <v>0.84027777777777779</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0.88263888888888886</v>
-      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="5">
-        <v>61</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
@@ -1249,22 +1225,12 @@
       <c r="A11" s="9">
         <v>5</v>
       </c>
-      <c r="B11" s="7">
-        <v>43888</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0.30555555555555552</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0.48958333333333331</v>
-      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="5">
-        <v>265</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
       <c r="H11" s="31"/>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
@@ -1273,22 +1239,12 @@
       <c r="A12" s="9">
         <v>6</v>
       </c>
-      <c r="B12" s="7">
-        <v>43889</v>
-      </c>
-      <c r="C12" s="8">
-        <v>0.85416666666666663</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0.90625</v>
-      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="5">
-        <v>75</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>53</v>
-      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
@@ -1297,25 +1253,13 @@
       <c r="A13" s="9">
         <v>7</v>
       </c>
-      <c r="B13" s="7">
-        <v>43890</v>
-      </c>
-      <c r="C13" s="8">
-        <v>0.32569444444444445</v>
-      </c>
-      <c r="D13" s="8">
-        <v>0.37152777777777773</v>
-      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="5">
-        <v>66</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="10"/>
     </row>
@@ -1324,19 +1268,11 @@
         <v>8</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="8">
-        <v>0.40625</v>
-      </c>
-      <c r="D14" s="8">
-        <v>0.41319444444444442</v>
-      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="5">
-        <v>10</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>56</v>
-      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
@@ -1345,20 +1281,12 @@
       <c r="A15" s="9">
         <v>9</v>
       </c>
-      <c r="B15" s="7">
-        <v>412785</v>
-      </c>
-      <c r="C15" s="8">
-        <v>0.46527777777777773</v>
-      </c>
-      <c r="D15" s="32">
-        <v>0.4826388888888889</v>
-      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="32"/>
       <c r="E15" s="6"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="6" t="s">
-        <v>57</v>
-      </c>
+      <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
@@ -1368,15 +1296,11 @@
         <v>10</v>
       </c>
       <c r="B16" s="7"/>
-      <c r="C16" s="8">
-        <v>0.69444444444444453</v>
-      </c>
+      <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="6"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="6" t="s">
-        <v>58</v>
-      </c>
+      <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
@@ -1419,7 +1343,7 @@
       <c r="E19" s="43"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>604</v>
+        <v>0</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>
@@ -1444,6 +1368,411 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8ACF002-C02F-4F6D-A9DF-5CDFC75330FF}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.36328125" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
+    <col min="6" max="6" width="6.54296875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="43.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.453125" customWidth="1"/>
+    <col min="10" max="10" width="3.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="46"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="47"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="49"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="51"/>
+      <c r="C4" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="53">
+        <v>43888</v>
+      </c>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="54"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="57"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="59"/>
+      <c r="C6" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="17">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7">
+        <v>43886</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5">
+        <v>25</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="38">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D8" s="38">
+        <v>0.75138888888888899</v>
+      </c>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40">
+        <v>32</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="39"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="37"/>
+      <c r="C9" s="8">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.8125</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5">
+        <v>70</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.88263888888888886</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5">
+        <v>61</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7">
+        <v>43888</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5">
+        <v>265</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="31"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="9">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7">
+        <v>43889</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.90625</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5">
+        <v>75</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="9">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7">
+        <v>43890</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.32569444444444445</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.37152777777777773</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5">
+        <v>66</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8">
+        <v>0.40625</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5">
+        <v>10</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="9">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7">
+        <v>412785</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="D15" s="32">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5">
+        <v>25</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="9">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0.95138888888888884</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5">
+        <v>370</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="9">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="23">
+        <v>12</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="30">
+        <f>SUM(F7:F18)</f>
+        <v>999</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4BA9E6-34DD-4C1C-AEEF-5A72BA45E7B5}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -1828,7 +2157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8DD912-1C37-45A7-B4D1-E4B8ABC30324}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -2189,7 +2518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CFBBF56-839A-44F9-A412-7D1F721290A1}">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -2612,7 +2941,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L19"/>
   <sheetViews>

</xml_diff>

<commit_message>
18-19. osa tehtud, KÕIK töötab
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC50EB25-23F7-4924-B6F4-0043CE57DDE1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA1D948-7F62-464B-BCEB-18F846511584}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,7 +215,7 @@
     <t>Kodutöö 13-17. osa</t>
   </si>
   <si>
-    <t>Eelmise kodutöö errorite eelimineerimine</t>
+    <t>Kodutöö 18-19. osa</t>
   </si>
 </sst>
 </file>
@@ -1167,11 +1167,15 @@
         <v>43892</v>
       </c>
       <c r="C7" s="8">
-        <v>0.36458333333333331</v>
-      </c>
-      <c r="D7" s="8"/>
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.77916666666666667</v>
+      </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5">
+        <v>120</v>
+      </c>
       <c r="G7" s="6" t="s">
         <v>59</v>
       </c>
@@ -1343,7 +1347,7 @@
       <c r="E19" s="43"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
sorted repo testid tehtud, kõik töötab
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA1D948-7F62-464B-BCEB-18F846511584}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5640C3-FF03-4248-9D50-3A9B283C4511}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="64">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -216,6 +216,18 @@
   </si>
   <si>
     <t>Kodutöö 18-19. osa</t>
+  </si>
+  <si>
+    <t>Kodutöö 20-23. osa</t>
+  </si>
+  <si>
+    <t>22.13</t>
+  </si>
+  <si>
+    <t>-30min + 43min juures pooleli</t>
+  </si>
+  <si>
+    <t>Kodutöö 23 lõpp -</t>
   </si>
 </sst>
 </file>
@@ -610,7 +622,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -676,6 +688,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="26" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1053,7 +1066,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1072,68 +1085,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="47"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="49"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="52" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="53">
+      <c r="G4" s="54">
         <v>43888</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="55"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="57"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="59"/>
+      <c r="B6" s="60"/>
       <c r="C6" s="34" t="s">
         <v>4</v>
       </c>
@@ -1187,13 +1200,25 @@
       <c r="A8" s="9">
         <v>2</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
+      <c r="B8" s="7">
+        <v>43893</v>
+      </c>
+      <c r="C8" s="38">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>61</v>
+      </c>
       <c r="E8" s="39"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
+      <c r="F8" s="40">
+        <v>285</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>62</v>
+      </c>
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
@@ -1201,12 +1226,18 @@
       <c r="A9" s="9">
         <v>3</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="37">
+        <v>43894</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="D9" s="8"/>
       <c r="E9" s="6"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
@@ -1338,16 +1369,16 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="44"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>120</v>
+        <v>405</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>
@@ -1395,68 +1426,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="47"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="49"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="52" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="53">
+      <c r="G4" s="54">
         <v>43888</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="55"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="57"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="59"/>
+      <c r="B6" s="60"/>
       <c r="C6" s="34" t="s">
         <v>4</v>
       </c>
@@ -1743,13 +1774,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="44"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>999</v>
@@ -1800,68 +1831,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="47"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="49"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="52" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="53">
+      <c r="G4" s="54">
         <v>43884</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="55"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="57"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="59"/>
+      <c r="B6" s="60"/>
       <c r="C6" s="34" t="s">
         <v>4</v>
       </c>
@@ -2128,13 +2159,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="44"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>912</v>
@@ -2185,68 +2216,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="47"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="49"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="52" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="53">
+      <c r="G4" s="54">
         <v>43877</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="55"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="57"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="59"/>
+      <c r="B6" s="60"/>
       <c r="C6" s="34" t="s">
         <v>4</v>
       </c>
@@ -2489,13 +2520,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="44"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>735</v>
@@ -2546,68 +2577,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="47"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="49"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="52" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="53">
+      <c r="G4" s="54">
         <v>43870</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="55"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="57"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="60"/>
+      <c r="B6" s="61"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -2912,13 +2943,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="44"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>1012</v>
@@ -2969,68 +3000,68 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="47"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="49"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="52" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="53">
+      <c r="G4" s="54">
         <v>43863</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="55"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="57"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" spans="1:12" s="3" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="60"/>
+      <c r="B6" s="61"/>
       <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
@@ -3293,13 +3324,13 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="44"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
         <v>920</v>

</xml_diff>

<commit_message>
25. osa tehtud, paging ka nüüd töötab, täiesti korras
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD859961-C5D7-41F3-9D37-1E89813AEAD0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604D7227-195E-41E6-8B91-D26D67E54C07}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="64">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>Kodutöö 23 lõpp - 24. osa</t>
+  </si>
+  <si>
+    <t>Kodutöö 25. osa</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1066,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1245,12 +1248,18 @@
       <c r="A10" s="9">
         <v>4</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="7">
+        <v>43897</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.46180555555555558</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="6"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>

</xml_diff>

<commit_message>
6. kodutöö + ajalogi
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elise\source\repos\Abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBEA888-74C9-447B-9180-2A851C504003}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344C83AA-E552-4B92-A593-E63336FB3D63}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -227,7 +227,7 @@
     <t>Kodutöö 23 lõpp - 24. osa</t>
   </si>
   <si>
-    <t>Kodutöö 25-26. osa</t>
+    <t>Kodutöö 25-27. osa</t>
   </si>
 </sst>
 </file>
@@ -1066,7 +1066,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1254,9 +1254,13 @@
       <c r="C10" s="8">
         <v>0.46180555555555558</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="8">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5">
+        <v>125</v>
+      </c>
       <c r="G10" s="6" t="s">
         <v>63</v>
       </c>
@@ -1386,7 +1390,7 @@
       <c r="E19" s="44"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>598</v>
+        <v>723</v>
       </c>
       <c r="G19" s="28" t="s">
         <v>35</v>

</xml_diff>